<commit_message>
Revert "Merge pull request #119 from hieu220413/VINH"
This reverts commit ec8613b784183dfaeab19584ea25d4444a058226, reversing
changes made to ee9cb4d9cd9fe52c499054b05b2a05e4313a6125.
</commit_message>
<xml_diff>
--- a/Screen-detail .xlsx
+++ b/Screen-detail .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chuyen nganh\SWP391\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chuyen nganh\SWP391\SWP_Dentist-Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046AAE9F-3B47-43DC-A157-C75CFB004651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0865A6A6-1C17-443D-8E9F-06B086C3DBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07E3085A-4D3C-47EB-BDFF-BC686D618F5D}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>Function/Screen</t>
   </si>
@@ -44,21 +36,42 @@
     <t>Promotion list</t>
   </si>
   <si>
+    <t>Promotion detail</t>
+  </si>
+  <si>
     <t>User login</t>
   </si>
   <si>
     <t>Register</t>
   </si>
   <si>
+    <t>Reset password</t>
+  </si>
+  <si>
     <t>Customer dashboard</t>
   </si>
   <si>
+    <t>Appointment list</t>
+  </si>
+  <si>
+    <t>Appointment detail</t>
+  </si>
+  <si>
     <t>User profile</t>
   </si>
   <si>
     <t>Booking appointment</t>
   </si>
   <si>
+    <t>Online payment</t>
+  </si>
+  <si>
+    <t>View invoice</t>
+  </si>
+  <si>
+    <t>Show list appointment history</t>
+  </si>
+  <si>
     <t>#</t>
   </si>
   <si>
@@ -83,12 +96,33 @@
     <t>Services list</t>
   </si>
   <si>
+    <t>Service detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Dentist dashboard</t>
   </si>
   <si>
     <t>Dentist</t>
   </si>
   <si>
+    <t>Achievement</t>
+  </si>
+  <si>
+    <t>Appointments list</t>
+  </si>
+  <si>
+    <t>Appointments detail</t>
+  </si>
+  <si>
+    <t>User list</t>
+  </si>
+  <si>
+    <t>Users detail</t>
+  </si>
+  <si>
     <t>Dentist detail</t>
   </si>
   <si>
@@ -98,7 +132,89 @@
     <t>Service list</t>
   </si>
   <si>
+    <t>Black list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction list </t>
+  </si>
+  <si>
+    <t>Transaction detail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Appointment list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment detail </t>
+  </si>
+  <si>
+    <t>Show promotion detail ( promotion ID , service ID, discount percentage, expired date, using date), complete introduction.</t>
+  </si>
+  <si>
+    <t>Search bar with name, price, rate filter 
++ Shown all services include brief introduction, price, rate and a button redirect user to complete service information.</t>
+  </si>
+  <si>
+    <t>Show service detail ( service ID , service Name, price, promotion ID - optional, rate) 
++ some high rate 
++ service feedback ( customerID, time, message, service ), complete introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show colorful background 
++ login ID, password input form 
++ reset input button 
++ forgot password button + register button. 
++ submit button which will do the authencation 
+Valid : redirect to the dashboard according to the account's role
+Invalid: show reason message </t>
+  </si>
+  <si>
+    <t>Show input email or phone depend on customer selection 
++ submit button which will send the authenticatioin message 
++ message ( error or success in sending the authentication message include new password to phone number / email  )</t>
+  </si>
+  <si>
+    <t>Search bar with meeting date  fileter 
++ Shown all appointment include time, meeting date, service name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show appointment detail ( meeting date, time, service name, service ID, dentist name, dentist ID, status ) 
++ cancel appointment button ( before 12 hours since customer books the appointment) 
++ message ( fail to cancel -reason - solution ) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show a booking input form include using combo box ( dentist name, service Name, time, payment method ), date.
++Show price after picking a serivce 
++ confirmation button ( require all the fields are not empty ) + message ( error or success ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show list appointment detail ( meeting date, time, service name, service ID, dentist name, dentist ID, status ) 
++ feedback forms include  service feedback ( message, rating ), dentist feedback ( message, rating)   
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show the number of case and case detail ( meeting date, time, service name, service ID, customer name, customer ID, status  ) in day or month or year 
++ feedback, rating of each case
+</t>
+  </si>
+  <si>
+    <t>Search bar with meeting date  fileter 
++ Show all appointment include time, meeting date, service name.</t>
+  </si>
+  <si>
+    <t>Show slider, top rate services and dentists, brief clinic's information, navbar with buttons redirect to other page.
++ Show slider information includes image and title (about services/dentist/clinic/sale). 
++ Show service information includes, image, name, price, brief introduction, click image will  redirect user to complete service information
++ Show dentist information includes name, brief introduction, rate and  a button redirect user to complete clinic information
++ Show brief clinic's information includes name, best achievement, time open close clinic and a button redirect user to complete clinic information</t>
+  </si>
+  <si>
+    <t>thêm promotion detail vào sql server</t>
+  </si>
+  <si>
+    <t>Search bar with name
++ Filter with service name, discount percentage, between activation and expired time 
++ Shown all promotion include brief introduction, discount percentage and a button redirect user to complete promotion information.</t>
   </si>
   <si>
     <t xml:space="preserve">Show register account form includes customer ID , user name, password, role, personal name, age, address, phone number, email 
@@ -106,239 +222,84 @@
 +  message ( success or error )   </t>
   </si>
   <si>
+    <t>Welcome message ( person name ) 
++ navbar with buttons redirect to all customer accessible pages 
++ coloful background 
++ up coming appointment or changing in appointment reminder message 
++ recommend some top rate service , sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show customer profile ( personal name, age, address,  phone number, Email ) and all this attribute can be editable with a button 
++ colorful background </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome message ( personal name ) 
++ show rating 
++ show navbar with buttons redirect to all dentist accessible pages 
++ coloful background 
++ show up coming appointment or changing in appointment reminder message + some top rate, feedback from customer 
++ show the number of appointment of the day.
+</t>
+  </si>
+  <si>
+    <t>Show appointment detail(meeting date, time, service name, service ID, customer name, customerID,status )</t>
+  </si>
+  <si>
+    <t>Search bar with personal name, age  filter
++ Show all customer includes personal name, age, phone number</t>
+  </si>
+  <si>
+    <t>Show Customer (customer ID, personal name, age, address, phone number, Email) 
++ Show customer detail ( customer ID, personal name, age, address, phone number, Email )
++ Ban button ( list the user account to backlist)</t>
+  </si>
+  <si>
+    <t>Show dentist detail ( dentist ID, personal name, age, rate ) 
++ some top good feedback ( high rating )
++ some bad feedback ( low rating )
++ delete account button</t>
+  </si>
+  <si>
+    <t>Show full detail of a specific transaction (transaction id, user name, service id, dentist id, price tag)</t>
+  </si>
+  <si>
+    <t>Show  a list of appointment has been confirmed before with CURD button</t>
+  </si>
+  <si>
+    <t>Show full detail of a appointment (user name, service id, dentist id, price tag, date, time, place)</t>
+  </si>
+  <si>
     <t>Admin dashboard</t>
   </si>
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>Search bar with name
-+ Filter with service name, discount percentage, between activation and expired time 
-+ Shown all promotion include brief introduction, discount percentage, expired date and a button redirect user to complete promotion information.
-+ Pop-up show promotion detail ( promotion ID , service ID, discount percentage, expired date, using date), complete introduction.</t>
-  </si>
-  <si>
-    <t>Search bar with years of work, rate filter
-+ Show all dentist include brief introduction, rate, years of work, speciality, name, image and a button redirect user to complete dentist information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show dentist detail ( dentist ID, personal name, age, rate, years of work,speciality,image,education,award ) 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show slider, top rate services and dentists, brief clinic's information, navbar with buttons redirect to other page.
-+ Show slider information includes image and title (about services/dentist/clinic/sale). 
-+ Show service information includes, image, name, price, brief introduction, click image will  redirect user to complete service information. 
-+ Show dentist information includes name, brief introduction, rate, image, click image will redirect user to complete dentist information. Button for booking (required login as customer)
-+ Show brief clinic's information includes name, phone, email, time open close clinic </t>
-  </si>
-  <si>
-    <t>Search bar with name, price, rate filter 
-+ Shown all services include brief introduction, price, rate and a button redirect user to complete service information.
-+ Pop-up  show service detail ( service ID , service Name, price, promotion ID - optional, rate) and button for booking (required login as customer)</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>Show a booking input form using schedule of dentist that customer chose to pick slot and service. 
-+ Show form to input symptom
-+ Show customer information (personal name, email, phone number), dentist (personal name, image, rate, speciality)
-+ Button to submit form, message (success or fail to book)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show colorful background 
-+ Login ID, password input form 
-+ Reset input button 
-+ Forgot password button + register button. 
-+ Submit button which will do the authencation 
-Valid : redirect to the dashboard according to the account's role
-Invalid: show reason message </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show customer information (personal name, email, phone number,address)
-+ Show dentist information (personal name, rate, years of experience)
-+ Show appointment (meeting date, slot), price
-+ Show service information (service name, price, discount percentage)
-+ Show check box for payment method (pay in cash or paypal) and term &amp; conditions 
-+ Button for submit form
-</t>
-  </si>
-  <si>
-    <t>Change password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show input form include old password, new password, confirm password
-+ Button to submimt form
-+ Message (success or fail to change password-reason)
-</t>
-  </si>
-  <si>
-    <t>Invoice list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show all invoice include invoice ID, appointment ID, employee ID, price, payment method, status
-+Button redirect user to view invoice detail
-</t>
-  </si>
-  <si>
-    <t>Invoice detail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show invoice  detail (  invoice ID, appointment ID, employee ID, price, payment method ) 
-+ Show employee name who create the invoice and customer (name, address) who receive the invoice.
-+ Show service (name, price), promotion discount percentage, total price.
-</t>
-  </si>
-  <si>
-    <t>Schedule update</t>
-  </si>
-  <si>
-    <t>Show all days in the week
-+ Show added slot  and button to add new slot for each day</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>Show customer feedback ( customer personal name, rate, message), appointment ID.</t>
-  </si>
-  <si>
-    <t>Dentist profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome message ( personal name ) 
-+ Show navbar with buttons redirect to all dentist accessible pages 
-+ Show sidebar with buttons redirect to all dentist accessible pages
-+ Show up coming appointment 
-+ Show checkout button, book button which will redirect dentist to booking page, View appointemnt detail button.
-+ Checkout pop-up include confirm button, input message (dentist note)  form.
-+ appointment detail pop-up include appointment ID, price, service Name, slot, meeting date
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome message ( person name ) 
-+ Navbar with buttons redirect to all customer accessible pages 
-+ SIdebar with buttons redirect to all customer accessible pages 
-+ Coloful background 
-+ Show all appointment ( divided into 3 different tabs ).  
-+ Show cancel appointment button ( before 2 hours since customer books the appointment) 
-+ Message ( fail to cancel -reason - solution ).
-+ Show Pay button which will redirect user to payment website.
-+ Show Feedback button which will display pop-up when customer click.
-+ Feedback Pop-up include rating and input message form. 
-+ Button view detail of the appointment (status, appointment date, dentist note, customer symptom, service, slot, price)
-+ Show appointment reminder message </t>
-  </si>
-  <si>
-    <t>Customer list</t>
-  </si>
-  <si>
-    <t>Show dentist profile ( personal name, speciality,  education, award, working excperience,gender,image, description ) and all attributes are editable 
-+ Button to submit form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show customer profile ( personal name, age, address,  phone number, Email,gender,image ) and all  attributes are editable 
- </t>
-  </si>
-  <si>
-    <t>Search bar with personal Name
-+ Show all customers using table with sort include customer ID , customer name, gender, age, email, status, phone.
-+ Show delete, restore, unrestrict,restrict button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Restrict Pop-up which will show confirm message and two button (cacncel, restrict)
-+ Unrestrict Pop-up which will show confirm message and two button (cacncel, unrestrict)</t>
-  </si>
-  <si>
-    <t>Search bar with service name
-+ Show all services using table with sort include service ID , service name, promotion ID, short description, price, status
-+ Show delete, restore, detail, edit button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Edit Pop-up which will show service detail using form (service ID , servicename, promotion ID, short description, long description,price) and all attributes are editable
-+ Detail Pop-up which will show service detail (service ID , servicename, promotion ID, short description, price, status, long description)
-+ Show message (success or fail-reason )</t>
-  </si>
-  <si>
-    <t>Search bar with personal Name
-+ Show all dentists using table with sort include dentist ID , dentist name, gender, speciality, rate, status
-+ Show delete, restore, detail, edit button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Edit Pop-up which will show dentist detail using form (dentist ID, personal name, age, rate, years of work,speciality,image,education,award) and all attributes are editable
-+ Detail Pop-up which will show dentist detail (dentist ID, personal name, age, rate, years of work,speciality,image,education,award,status)
-+ Show message (success or fail-reason)</t>
-  </si>
-  <si>
-    <t>Search bar with expired date
-+ Show all promotions using table with sort include promotion ID , promotion name, short description, discount percentage, expired date, status
-+ Show delete, restore, detail, edit button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Edit Pop-up which will show promotion detail using form ( promotion ID , promotion name, short description, discount percentage, expired date, long description) and all attributes are editable
-+ Detail Pop-up which will show service detail (promotion ID , promotion name, short description, discount percentage, expired date, status, long description)
-+ Show message (success or fail-reason )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search bar with meeting date
-+ Show all appointment using table with sort include appointment ID , promotion name, customer name, dentist name, appointment date, slot, status, dentist confirm, payment confirm
-+ Show detail button.
-+ Detail Pop-up which will show appointment detail (appointment ID , promotion name, customer name, dentist name, appointment date, slot, service name, status, dentist confirm, payment confirm)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feedback list </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search bar with rate
-+ Show all feedback using table with sort include feedback ID, customer name, dentist name, rate, comment, status
-+ Show detail, delete, restore button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Detail Pop-up which will show feedback detail (feedback ID, customer name, dentist name, rate, comment, status)
-</t>
-  </si>
-  <si>
     <t>Welcome message ( personal name ) 
-+ show  sidebar with buttons redirect to all Admin accessible pages 
++ show  buttons redirect to all Admin accessible pages 
 + coloful background 
 + show table, graphic about the profit of clinic in day or month or year 
-+ show top services and dentists ( judging by rating and pick rate )
-+ show top customer ( judging by spending )</t>
-  </si>
-  <si>
-    <t>Employee dashboard</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>Show navbar with buttons redirect to all employee accessible pages
-+ Show sidebar with buttons redirect to all employee accessible pages 
-+ Show number of patient, number of appointments in the week, number of today appointments
-+ Show table with 4 tabs (today appointments, weekly appointments, upcoming appointments, archive) which display appointment ID, customer name, dentist name, appointment date, appointment status.
-+ Show Delete button in all tabs except archive.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)</t>
-  </si>
-  <si>
-    <t>Show table with 3 tabs (Checkin, In progress, finished) which display appointment ID, customer name, dentist name, appointment date, appointment status.
-+ Show View detail button in Checkin tab
-+ View detail Pop-up of checkin tab will show appointment date, dentist not, customer symptom. service name, slot, price and checkin button 
-+ Show View detail button in In Progess tab
-+ View detail Pop-up of in In Progess tab will show appointment date, dentist not, customer symptom. service name, slot, price, payment status and view invoice button which will redirect user to invoice page</t>
-  </si>
-  <si>
-    <t>Show invoice  detail (  invoice ID, appointment ID, employee ID, price, payment method, payment status) 
-+ Show service (name, price), promotion discount percentage, total
-+ Show customer name, address (who receives the invoice)
-+ Show confirm checkout button
-+ Confirm checkout Pop-up which will show confirm message and one button (checkout now)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show feedback list include Feedback ID, appointment ID, rate, message for dentist, status 
-+ Show accept, reject button.
-</t>
++ show top 3 services and dentists ( judging by rating and pick rate )
++ show top 3 customer ( judging by spending )</t>
+  </si>
+  <si>
+    <t>Search bar with personal name, age  filter
++ Show all customer includes personal name, age, rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show list of users in database with search bar by name, age. Show another list of users in blacklist with detail and a button [remove from blacklist]. </t>
+  </si>
+  <si>
+    <t>Show service detail ( service ID, service name, price, number of customer have used service, rating,
+description )</t>
+  </si>
+  <si>
+    <t>Search bar with service name, price  filter
++Show list of service including name of service name, number of customer have used service, rating, price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search bar with serivice ID , date , customer ID 
+Show a list of transactions which are made during the active hours - with search bar (by user name, transaction id) </t>
   </si>
 </sst>
 </file>
@@ -400,10 +361,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,43 +680,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FAC205-8EFD-46BB-AFDB-14A75F955239}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="6"/>
+    <col min="1" max="1" width="8.6640625" style="7"/>
     <col min="2" max="2" width="29.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1"/>
     <col min="6" max="6" width="93.33203125" customWidth="1"/>
     <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -763,16 +724,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -780,29 +741,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -811,32 +774,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -845,15 +810,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -862,379 +827,444 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="7" t="s">
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reset to ec8613b second try
</commit_message>
<xml_diff>
--- a/Screen-detail .xlsx
+++ b/Screen-detail .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chuyen nganh\SWP391\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chuyen nganh\SWP391\SWP_Dentist-Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046AAE9F-3B47-43DC-A157-C75CFB004651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0865A6A6-1C17-443D-8E9F-06B086C3DBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07E3085A-4D3C-47EB-BDFF-BC686D618F5D}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>Function/Screen</t>
   </si>
@@ -44,21 +36,42 @@
     <t>Promotion list</t>
   </si>
   <si>
+    <t>Promotion detail</t>
+  </si>
+  <si>
     <t>User login</t>
   </si>
   <si>
     <t>Register</t>
   </si>
   <si>
+    <t>Reset password</t>
+  </si>
+  <si>
     <t>Customer dashboard</t>
   </si>
   <si>
+    <t>Appointment list</t>
+  </si>
+  <si>
+    <t>Appointment detail</t>
+  </si>
+  <si>
     <t>User profile</t>
   </si>
   <si>
     <t>Booking appointment</t>
   </si>
   <si>
+    <t>Online payment</t>
+  </si>
+  <si>
+    <t>View invoice</t>
+  </si>
+  <si>
+    <t>Show list appointment history</t>
+  </si>
+  <si>
     <t>#</t>
   </si>
   <si>
@@ -83,12 +96,33 @@
     <t>Services list</t>
   </si>
   <si>
+    <t>Service detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Dentist dashboard</t>
   </si>
   <si>
     <t>Dentist</t>
   </si>
   <si>
+    <t>Achievement</t>
+  </si>
+  <si>
+    <t>Appointments list</t>
+  </si>
+  <si>
+    <t>Appointments detail</t>
+  </si>
+  <si>
+    <t>User list</t>
+  </si>
+  <si>
+    <t>Users detail</t>
+  </si>
+  <si>
     <t>Dentist detail</t>
   </si>
   <si>
@@ -98,7 +132,89 @@
     <t>Service list</t>
   </si>
   <si>
+    <t>Black list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction list </t>
+  </si>
+  <si>
+    <t>Transaction detail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Appointment list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment detail </t>
+  </si>
+  <si>
+    <t>Show promotion detail ( promotion ID , service ID, discount percentage, expired date, using date), complete introduction.</t>
+  </si>
+  <si>
+    <t>Search bar with name, price, rate filter 
++ Shown all services include brief introduction, price, rate and a button redirect user to complete service information.</t>
+  </si>
+  <si>
+    <t>Show service detail ( service ID , service Name, price, promotion ID - optional, rate) 
++ some high rate 
++ service feedback ( customerID, time, message, service ), complete introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show colorful background 
++ login ID, password input form 
++ reset input button 
++ forgot password button + register button. 
++ submit button which will do the authencation 
+Valid : redirect to the dashboard according to the account's role
+Invalid: show reason message </t>
+  </si>
+  <si>
+    <t>Show input email or phone depend on customer selection 
++ submit button which will send the authenticatioin message 
++ message ( error or success in sending the authentication message include new password to phone number / email  )</t>
+  </si>
+  <si>
+    <t>Search bar with meeting date  fileter 
++ Shown all appointment include time, meeting date, service name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show appointment detail ( meeting date, time, service name, service ID, dentist name, dentist ID, status ) 
++ cancel appointment button ( before 12 hours since customer books the appointment) 
++ message ( fail to cancel -reason - solution ) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show a booking input form include using combo box ( dentist name, service Name, time, payment method ), date.
++Show price after picking a serivce 
++ confirmation button ( require all the fields are not empty ) + message ( error or success ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show list appointment detail ( meeting date, time, service name, service ID, dentist name, dentist ID, status ) 
++ feedback forms include  service feedback ( message, rating ), dentist feedback ( message, rating)   
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show the number of case and case detail ( meeting date, time, service name, service ID, customer name, customer ID, status  ) in day or month or year 
++ feedback, rating of each case
+</t>
+  </si>
+  <si>
+    <t>Search bar with meeting date  fileter 
++ Show all appointment include time, meeting date, service name.</t>
+  </si>
+  <si>
+    <t>Show slider, top rate services and dentists, brief clinic's information, navbar with buttons redirect to other page.
++ Show slider information includes image and title (about services/dentist/clinic/sale). 
++ Show service information includes, image, name, price, brief introduction, click image will  redirect user to complete service information
++ Show dentist information includes name, brief introduction, rate and  a button redirect user to complete clinic information
++ Show brief clinic's information includes name, best achievement, time open close clinic and a button redirect user to complete clinic information</t>
+  </si>
+  <si>
+    <t>thêm promotion detail vào sql server</t>
+  </si>
+  <si>
+    <t>Search bar with name
++ Filter with service name, discount percentage, between activation and expired time 
++ Shown all promotion include brief introduction, discount percentage and a button redirect user to complete promotion information.</t>
   </si>
   <si>
     <t xml:space="preserve">Show register account form includes customer ID , user name, password, role, personal name, age, address, phone number, email 
@@ -106,239 +222,84 @@
 +  message ( success or error )   </t>
   </si>
   <si>
+    <t>Welcome message ( person name ) 
++ navbar with buttons redirect to all customer accessible pages 
++ coloful background 
++ up coming appointment or changing in appointment reminder message 
++ recommend some top rate service , sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show customer profile ( personal name, age, address,  phone number, Email ) and all this attribute can be editable with a button 
++ colorful background </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome message ( personal name ) 
++ show rating 
++ show navbar with buttons redirect to all dentist accessible pages 
++ coloful background 
++ show up coming appointment or changing in appointment reminder message + some top rate, feedback from customer 
++ show the number of appointment of the day.
+</t>
+  </si>
+  <si>
+    <t>Show appointment detail(meeting date, time, service name, service ID, customer name, customerID,status )</t>
+  </si>
+  <si>
+    <t>Search bar with personal name, age  filter
++ Show all customer includes personal name, age, phone number</t>
+  </si>
+  <si>
+    <t>Show Customer (customer ID, personal name, age, address, phone number, Email) 
++ Show customer detail ( customer ID, personal name, age, address, phone number, Email )
++ Ban button ( list the user account to backlist)</t>
+  </si>
+  <si>
+    <t>Show dentist detail ( dentist ID, personal name, age, rate ) 
++ some top good feedback ( high rating )
++ some bad feedback ( low rating )
++ delete account button</t>
+  </si>
+  <si>
+    <t>Show full detail of a specific transaction (transaction id, user name, service id, dentist id, price tag)</t>
+  </si>
+  <si>
+    <t>Show  a list of appointment has been confirmed before with CURD button</t>
+  </si>
+  <si>
+    <t>Show full detail of a appointment (user name, service id, dentist id, price tag, date, time, place)</t>
+  </si>
+  <si>
     <t>Admin dashboard</t>
   </si>
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>Search bar with name
-+ Filter with service name, discount percentage, between activation and expired time 
-+ Shown all promotion include brief introduction, discount percentage, expired date and a button redirect user to complete promotion information.
-+ Pop-up show promotion detail ( promotion ID , service ID, discount percentage, expired date, using date), complete introduction.</t>
-  </si>
-  <si>
-    <t>Search bar with years of work, rate filter
-+ Show all dentist include brief introduction, rate, years of work, speciality, name, image and a button redirect user to complete dentist information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show dentist detail ( dentist ID, personal name, age, rate, years of work,speciality,image,education,award ) 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show slider, top rate services and dentists, brief clinic's information, navbar with buttons redirect to other page.
-+ Show slider information includes image and title (about services/dentist/clinic/sale). 
-+ Show service information includes, image, name, price, brief introduction, click image will  redirect user to complete service information. 
-+ Show dentist information includes name, brief introduction, rate, image, click image will redirect user to complete dentist information. Button for booking (required login as customer)
-+ Show brief clinic's information includes name, phone, email, time open close clinic </t>
-  </si>
-  <si>
-    <t>Search bar with name, price, rate filter 
-+ Shown all services include brief introduction, price, rate and a button redirect user to complete service information.
-+ Pop-up  show service detail ( service ID , service Name, price, promotion ID - optional, rate) and button for booking (required login as customer)</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>Show a booking input form using schedule of dentist that customer chose to pick slot and service. 
-+ Show form to input symptom
-+ Show customer information (personal name, email, phone number), dentist (personal name, image, rate, speciality)
-+ Button to submit form, message (success or fail to book)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show colorful background 
-+ Login ID, password input form 
-+ Reset input button 
-+ Forgot password button + register button. 
-+ Submit button which will do the authencation 
-Valid : redirect to the dashboard according to the account's role
-Invalid: show reason message </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show customer information (personal name, email, phone number,address)
-+ Show dentist information (personal name, rate, years of experience)
-+ Show appointment (meeting date, slot), price
-+ Show service information (service name, price, discount percentage)
-+ Show check box for payment method (pay in cash or paypal) and term &amp; conditions 
-+ Button for submit form
-</t>
-  </si>
-  <si>
-    <t>Change password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show input form include old password, new password, confirm password
-+ Button to submimt form
-+ Message (success or fail to change password-reason)
-</t>
-  </si>
-  <si>
-    <t>Invoice list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show all invoice include invoice ID, appointment ID, employee ID, price, payment method, status
-+Button redirect user to view invoice detail
-</t>
-  </si>
-  <si>
-    <t>Invoice detail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show invoice  detail (  invoice ID, appointment ID, employee ID, price, payment method ) 
-+ Show employee name who create the invoice and customer (name, address) who receive the invoice.
-+ Show service (name, price), promotion discount percentage, total price.
-</t>
-  </si>
-  <si>
-    <t>Schedule update</t>
-  </si>
-  <si>
-    <t>Show all days in the week
-+ Show added slot  and button to add new slot for each day</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>Show customer feedback ( customer personal name, rate, message), appointment ID.</t>
-  </si>
-  <si>
-    <t>Dentist profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome message ( personal name ) 
-+ Show navbar with buttons redirect to all dentist accessible pages 
-+ Show sidebar with buttons redirect to all dentist accessible pages
-+ Show up coming appointment 
-+ Show checkout button, book button which will redirect dentist to booking page, View appointemnt detail button.
-+ Checkout pop-up include confirm button, input message (dentist note)  form.
-+ appointment detail pop-up include appointment ID, price, service Name, slot, meeting date
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome message ( person name ) 
-+ Navbar with buttons redirect to all customer accessible pages 
-+ SIdebar with buttons redirect to all customer accessible pages 
-+ Coloful background 
-+ Show all appointment ( divided into 3 different tabs ).  
-+ Show cancel appointment button ( before 2 hours since customer books the appointment) 
-+ Message ( fail to cancel -reason - solution ).
-+ Show Pay button which will redirect user to payment website.
-+ Show Feedback button which will display pop-up when customer click.
-+ Feedback Pop-up include rating and input message form. 
-+ Button view detail of the appointment (status, appointment date, dentist note, customer symptom, service, slot, price)
-+ Show appointment reminder message </t>
-  </si>
-  <si>
-    <t>Customer list</t>
-  </si>
-  <si>
-    <t>Show dentist profile ( personal name, speciality,  education, award, working excperience,gender,image, description ) and all attributes are editable 
-+ Button to submit form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show customer profile ( personal name, age, address,  phone number, Email,gender,image ) and all  attributes are editable 
- </t>
-  </si>
-  <si>
-    <t>Search bar with personal Name
-+ Show all customers using table with sort include customer ID , customer name, gender, age, email, status, phone.
-+ Show delete, restore, unrestrict,restrict button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Restrict Pop-up which will show confirm message and two button (cacncel, restrict)
-+ Unrestrict Pop-up which will show confirm message and two button (cacncel, unrestrict)</t>
-  </si>
-  <si>
-    <t>Search bar with service name
-+ Show all services using table with sort include service ID , service name, promotion ID, short description, price, status
-+ Show delete, restore, detail, edit button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Edit Pop-up which will show service detail using form (service ID , servicename, promotion ID, short description, long description,price) and all attributes are editable
-+ Detail Pop-up which will show service detail (service ID , servicename, promotion ID, short description, price, status, long description)
-+ Show message (success or fail-reason )</t>
-  </si>
-  <si>
-    <t>Search bar with personal Name
-+ Show all dentists using table with sort include dentist ID , dentist name, gender, speciality, rate, status
-+ Show delete, restore, detail, edit button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Edit Pop-up which will show dentist detail using form (dentist ID, personal name, age, rate, years of work,speciality,image,education,award) and all attributes are editable
-+ Detail Pop-up which will show dentist detail (dentist ID, personal name, age, rate, years of work,speciality,image,education,award,status)
-+ Show message (success or fail-reason)</t>
-  </si>
-  <si>
-    <t>Search bar with expired date
-+ Show all promotions using table with sort include promotion ID , promotion name, short description, discount percentage, expired date, status
-+ Show delete, restore, detail, edit button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Edit Pop-up which will show promotion detail using form ( promotion ID , promotion name, short description, discount percentage, expired date, long description) and all attributes are editable
-+ Detail Pop-up which will show service detail (promotion ID , promotion name, short description, discount percentage, expired date, status, long description)
-+ Show message (success or fail-reason )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search bar with meeting date
-+ Show all appointment using table with sort include appointment ID , promotion name, customer name, dentist name, appointment date, slot, status, dentist confirm, payment confirm
-+ Show detail button.
-+ Detail Pop-up which will show appointment detail (appointment ID , promotion name, customer name, dentist name, appointment date, slot, service name, status, dentist confirm, payment confirm)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feedback list </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search bar with rate
-+ Show all feedback using table with sort include feedback ID, customer name, dentist name, rate, comment, status
-+ Show detail, delete, restore button.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)
-+ Restore Pop-up which will show confirm message and two button (cancel, restore)
-+ Detail Pop-up which will show feedback detail (feedback ID, customer name, dentist name, rate, comment, status)
-</t>
-  </si>
-  <si>
     <t>Welcome message ( personal name ) 
-+ show  sidebar with buttons redirect to all Admin accessible pages 
++ show  buttons redirect to all Admin accessible pages 
 + coloful background 
 + show table, graphic about the profit of clinic in day or month or year 
-+ show top services and dentists ( judging by rating and pick rate )
-+ show top customer ( judging by spending )</t>
-  </si>
-  <si>
-    <t>Employee dashboard</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>Show navbar with buttons redirect to all employee accessible pages
-+ Show sidebar with buttons redirect to all employee accessible pages 
-+ Show number of patient, number of appointments in the week, number of today appointments
-+ Show table with 4 tabs (today appointments, weekly appointments, upcoming appointments, archive) which display appointment ID, customer name, dentist name, appointment date, appointment status.
-+ Show Delete button in all tabs except archive.
-+ Delete Pop-up which will show confirm message and two button (cancel, delete)</t>
-  </si>
-  <si>
-    <t>Show table with 3 tabs (Checkin, In progress, finished) which display appointment ID, customer name, dentist name, appointment date, appointment status.
-+ Show View detail button in Checkin tab
-+ View detail Pop-up of checkin tab will show appointment date, dentist not, customer symptom. service name, slot, price and checkin button 
-+ Show View detail button in In Progess tab
-+ View detail Pop-up of in In Progess tab will show appointment date, dentist not, customer symptom. service name, slot, price, payment status and view invoice button which will redirect user to invoice page</t>
-  </si>
-  <si>
-    <t>Show invoice  detail (  invoice ID, appointment ID, employee ID, price, payment method, payment status) 
-+ Show service (name, price), promotion discount percentage, total
-+ Show customer name, address (who receives the invoice)
-+ Show confirm checkout button
-+ Confirm checkout Pop-up which will show confirm message and one button (checkout now)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show feedback list include Feedback ID, appointment ID, rate, message for dentist, status 
-+ Show accept, reject button.
-</t>
++ show top 3 services and dentists ( judging by rating and pick rate )
++ show top 3 customer ( judging by spending )</t>
+  </si>
+  <si>
+    <t>Search bar with personal name, age  filter
++ Show all customer includes personal name, age, rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show list of users in database with search bar by name, age. Show another list of users in blacklist with detail and a button [remove from blacklist]. </t>
+  </si>
+  <si>
+    <t>Show service detail ( service ID, service name, price, number of customer have used service, rating,
+description )</t>
+  </si>
+  <si>
+    <t>Search bar with service name, price  filter
++Show list of service including name of service name, number of customer have used service, rating, price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search bar with serivice ID , date , customer ID 
+Show a list of transactions which are made during the active hours - with search bar (by user name, transaction id) </t>
   </si>
 </sst>
 </file>
@@ -400,10 +361,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,43 +680,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FAC205-8EFD-46BB-AFDB-14A75F955239}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="6"/>
+    <col min="1" max="1" width="8.6640625" style="7"/>
     <col min="2" max="2" width="29.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1"/>
     <col min="6" max="6" width="93.33203125" customWidth="1"/>
     <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -763,16 +724,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -780,29 +741,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -811,32 +774,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -845,15 +810,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -862,379 +827,444 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="7" t="s">
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>